<commit_message>
Fixed the black patch issue occuring in updated Chrome browser Updated BVTs
</commit_message>
<xml_diff>
--- a/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Cylindrical Gauge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84CFB1A-0B44-47EF-B961-D3464FBB26E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="7965" xr2:uid="{6CA504DF-EEC1-406B-8211-12A36D5258A3}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>S no</t>
   </si>
@@ -48,151 +49,227 @@
     <t>Display basic Cylindrical Gauge</t>
   </si>
   <si>
-    <t>Drag 'Data' in 'Values' field</t>
-  </si>
-  <si>
     <t>Configurations</t>
   </si>
   <si>
-    <t>Update fill, border, max, min, tick bar, tick color, display units and decimal value for ticks</t>
-  </si>
-  <si>
-    <t>1. Fill color will be set to 'red'
-2. Border color will be set to 'grey'
-3. Max will be set to '150'
-4. Min will be set to '10'
-5. Tick bar will be set to hidden
-6. Tick color will be set to 'brown'
-7.Tick value will be set to like '40K'
-8. Tick value will be set to like '40.00K'</t>
-  </si>
-  <si>
     <t>Data Label</t>
   </si>
   <si>
     <t>Update label position, color, display unit and decimal places for data label</t>
   </si>
   <si>
-    <t>1. Go to formatting pane
+    <t># </t>
+  </si>
+  <si>
+    <t>Checklist Point </t>
+  </si>
+  <si>
+    <t>Yes/No </t>
+  </si>
+  <si>
+    <t>Have no console errors in IE 11, Edge, Chrome and Firefox browsers by having query string "unmin = true" in the URL? </t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Does visual render properly on resizing? </t>
+  </si>
+  <si>
+    <t>Does visual render properly on increasing title/data labels font sizes? </t>
+  </si>
+  <si>
+    <t>Does visual render properly on PBI desktop and PBI service? </t>
+  </si>
+  <si>
+    <t>Is Selection and Highlight feature working properly by selecting the slice of the visual when we have multiple other visuals along with our visual present in the report? </t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Does visual work properly on changing format in Modelling ribbon? Should match with other visuals behaviour </t>
+  </si>
+  <si>
+    <t>Have we handled Zero and NULL values for axis/data values and labels properly? Should match with other visuals behaviour.  </t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Have we used default PBI methods? </t>
+  </si>
+  <si>
+    <t>Does visual format values by default (K, M, B)? </t>
+  </si>
+  <si>
+    <t>Are visual custom properties working or not? </t>
+  </si>
+  <si>
+    <t>Are visual custom properties On/Off working or not? </t>
+  </si>
+  <si>
+    <t>Does visual render properly in Windows, Android, iPhone and iPad devices? </t>
+  </si>
+  <si>
+    <t>Is sorting functionality working fine by selecting different Sort by values and Order by values in Visual? </t>
+  </si>
+  <si>
+    <t>Is visual colors options working fine? </t>
+  </si>
+  <si>
+    <t>Is visual tested on msit.powerbi.com, app.powerbi.com, and dxt.powerbi.com services?  </t>
+  </si>
+  <si>
+    <t>Is the entire functionality set executed and 0 errors reported for </t>
+  </si>
+  <si>
+    <t>1. query string parameters “unmin=true&amp;approvedResourcesEnabled=false” </t>
+  </si>
+  <si>
+    <t>2. Query string parameters "sandboxVisualsEnabled=1&amp;approvedResourcesEnabled=false&amp;unmin=true" </t>
+  </si>
+  <si>
+    <t>Does visual work correctly after pinning visual to dashboard and pinning live report with the custom visual to the dashboard  </t>
+  </si>
+  <si>
+    <t>Does Custom properties followed proper casing?  </t>
+  </si>
+  <si>
+    <t>e.g., Data colors - Correct </t>
+  </si>
+  <si>
+    <t>         Data Colors - Incorrect  </t>
+  </si>
+  <si>
+    <t>Refer built-in charts for more details. </t>
+  </si>
+  <si>
+    <t>Does visual fully utilized the available chart area? </t>
+  </si>
+  <si>
+    <t>Does visual legends adjusted on resizing? </t>
+  </si>
+  <si>
+    <t>Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Go to formatting pane
 2. Go to 'Configurations' option
-3. Update 'Fill color' to 'red'
-4. Update 'Border color' to 'grey'
-5. Update 'Max' to '150'
-6. Update 'Min' to '10'
-7. Switch toggle of 'Tick Bar' OFF
-8. Update 'Tick color' to 'brown'
-9. Update 'Display units' to 'Thousand'
-10. Update 'Decimal value' to '2'</t>
+3. Update 'Lower Gradient fill' to 'light blue'
+4. Update 'Upper Gradient fill' to 'light blue'
+5. Update 'Lower Ellipse fill' to 'dark blue'
+6. Update 'Upper Ellipse fill' to 'dark blue'
+7. Update 'Background fill' to 'grey'
+8.  Update  'Animation time' to '5'
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Lower Gradient color will be set to 'light blue'
+2. Upper Gradient color will be set to 'light blue'
+3. Lower Ellipse color will be set to 'dark blue'
+4. Upper Ellipse color will be set to 'dark blue'
+5. Background color will be set to 'grey'
+</t>
+  </si>
+  <si>
+    <t>1. Switch toggle of 'Scale' to 'OFF'
+2. Switch toggle of 'Scale' to 'ON'
+3.Update 'Scale Color' to 'blue'
+4. Update 'Scale Position' to 'left'
+5. Update 'Font Family' to 'Arial'
+6. Update 'Font Size' to '16'
+7. Update 'Display units' to 'Thousand'
+8. Update 'Decimal value' to '2'</t>
+  </si>
+  <si>
+    <t>1. Max will be set to '800000'
+2. Min will be set to '100000'
+3. Target color will be set to 'Red'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Greater will be set to '500K'
+2. Less will be set to '300K'
+3. Greater Color will be updated to 'brown'
+4. Less Color will be updated  to 'red'
+</t>
+  </si>
+  <si>
+    <t>1. Scale will get hidden
+2. Scale will become visible and its color will be set to 'blue'
+3. Scale will be positioned to 'left'
+4. Font will be set to 'Arial'
+5. Font Size will be set to '16'
+6. Scale values will be represented in thousands and look like '400K'
+7. Decimal places will be set to 2 and values will look like '400.00K</t>
   </si>
   <si>
     <t>1. Go to formatting pane
 2. Go to 'Data label' option
-3. Update 'Label Position' to 'Inside'
-4. Update 'Text Size' to '27'
-5. Update color to 'blue' 
+3. Update 'Label Position' to 'Within the Cylinder'
+4. Update 'Font Size' to '27'
+5. Update color to 'red' 
 6. Update display unit to 'Thousand'
 7. Update decimal value  to '1'</t>
   </si>
   <si>
-    <t xml:space="preserve">
-1. Label position will be set Inside
+    <t>Update fill, border, max, min, target range, scale, display units and decimal value for scale</t>
+  </si>
+  <si>
+    <t>1. Label position will be set Inside
 2. Text size will be set to '27px' 
-3. Data label font color will be set to 'Blue'
-4. Text will be formatted like '50K'
-5. Text will be formatted like '50.0K'</t>
-  </si>
-  <si>
-    <t># </t>
-  </si>
-  <si>
-    <t>Checklist Point </t>
-  </si>
-  <si>
-    <t>Yes/No </t>
-  </si>
-  <si>
-    <t>Have no console errors in IE 11, Edge, Chrome and Firefox browsers by having query string "unmin = true" in the URL? </t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Does visual render properly on resizing? </t>
-  </si>
-  <si>
-    <t>Does visual render properly on increasing title/data labels font sizes? </t>
-  </si>
-  <si>
-    <t>Does visual render properly on PBI desktop and PBI service? </t>
-  </si>
-  <si>
-    <t>Is Selection and Highlight feature working properly by selecting the slice of the visual when we have multiple other visuals along with our visual present in the report? </t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Does visual work properly on changing format in Modelling ribbon? Should match with other visuals behaviour </t>
-  </si>
-  <si>
-    <t>Have we handled Zero and NULL values for axis/data values and labels properly? Should match with other visuals behaviour.  </t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Have we used default PBI methods? </t>
-  </si>
-  <si>
-    <t>Does visual format values by default (K, M, B)? </t>
-  </si>
-  <si>
-    <t>Are visual custom properties working or not? </t>
-  </si>
-  <si>
-    <t>Are visual custom properties On/Off working or not? </t>
-  </si>
-  <si>
-    <t>Does visual render properly in Windows, Android, iPhone and iPad devices? </t>
-  </si>
-  <si>
-    <t>Is sorting functionality working fine by selecting different Sort by values and Order by values in Visual? </t>
-  </si>
-  <si>
-    <t>Is visual colors options working fine? </t>
-  </si>
-  <si>
-    <t>Is visual tested on msit.powerbi.com, app.powerbi.com, and dxt.powerbi.com services?  </t>
-  </si>
-  <si>
-    <t>Is the entire functionality set executed and 0 errors reported for </t>
-  </si>
-  <si>
-    <t>1. query string parameters “unmin=true&amp;approvedResourcesEnabled=false” </t>
-  </si>
-  <si>
-    <t>2. Query string parameters "sandboxVisualsEnabled=1&amp;approvedResourcesEnabled=false&amp;unmin=true" </t>
-  </si>
-  <si>
-    <t>Does visual work correctly after pinning visual to dashboard and pinning live report with the custom visual to the dashboard  </t>
-  </si>
-  <si>
-    <t>Does Custom properties followed proper casing?  </t>
-  </si>
-  <si>
-    <t>e.g., Data colors - Correct </t>
-  </si>
-  <si>
-    <t>         Data Colors - Incorrect  </t>
-  </si>
-  <si>
-    <t>Refer built-in charts for more details. </t>
-  </si>
-  <si>
-    <t>Does visual fully utilized the available chart area? </t>
-  </si>
-  <si>
-    <t>Does visual legends adjusted on resizing? </t>
+3. Data label font color will be set to 'Red'
+4. Text will be formatted like '374K'
+5. Text will be formatted like '374.3K'</t>
+  </si>
+  <si>
+    <t>1. Drag 'Revenue' in 'Actual Value' field
+2. Drag 'Target' in 'Target Value' field
+3. Update 'Max' to '800000'
+4. Update 'Min' to '100000'
+5. Update 'Target Color' to 'red'</t>
+  </si>
+  <si>
+    <t>1. Drag 'Revenue' in 'Actual Value' field
+2. Drag 'Target' in 'Target Value' field
+3. Drag 'Min Revenue' to 'Min' field
+4. Drag 'Max Revenue' to 'Max' field</t>
+  </si>
+  <si>
+    <t>1. Drag 'Revenue' in 'Actual Value' field
+2. Drag 'Target' in 'Target Value' field
+3. Drag 'Min Revenue' to 'Min' field
+4. Drag 'Max Revenue' to 'Max' field
+5. Switch toggle of 'Target Range' to 'ON'
+6. Update 'Greater' to '500000'
+7. Update 'Less' to '300000'
+8. Update 'Greater Color' to 'brown'
+9. Update 'Less Color' to 'red'</t>
+  </si>
+  <si>
+    <t>Update zone 1, zone 2 , zone 3 and zone 4 values and upate their color</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Switch the toggle of 'Zones' to 'ON'
+3. Update 'Zone 1' value to '378000'
+4. Update 'Zone 1' color to 'yellow'
+5. Update 'Zone 2' value to '502000'
+6. Update 'Zone 2' color to 'green'
+7. Update 'Zone 3' value to '627000'
+8. Update 'Zone 3' color to 'orange'
+9. Update 'Zone 4' value to '748500'
+10. Update 'Zone 4' color to 'red'</t>
+  </si>
+  <si>
+    <t>1. Zone 1 value will be set to '378000'
+2. Zone 1 color will be set to 'yellow'
+3. Zone 1 value will be set to '378000'
+4. Zone 1 color will be set to 'yellow'
+5. Zone 1 value will be set to '378000'
+6. Zone 1 color will be set to 'yellow'
+7. Zone 1 value will be set to '378000'
+8. Zone 1 color will be set to 'yellow'</t>
   </si>
 </sst>
 </file>
@@ -257,20 +334,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,19 +681,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89ECC3-919A-4CE0-A09A-814B2A8DA1B6}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="49.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="33.85546875" style="9" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -605,68 +701,112 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="8"/>
+      <c r="D4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+      <c r="D5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
+      <c r="D7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -688,14 +828,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>18</v>
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -703,10 +843,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -714,10 +854,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,10 +865,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -736,10 +876,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -747,10 +887,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -758,10 +898,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -769,10 +909,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -780,10 +920,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -791,10 +931,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,10 +942,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -813,10 +953,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -824,10 +964,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -835,10 +975,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,10 +986,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -857,10 +997,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,20 +1008,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -889,10 +1029,10 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,25 +1040,25 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +1066,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +1077,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed metadata and categorical index issue
</commit_message>
<xml_diff>
--- a/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/CylindricalGauge/CylindricalGaugeByMAQSoftwareChecklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAQUser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Gitlab_Repos\documents\Published\CylindricalGauge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84CFB1A-0B44-47EF-B961-D3464FBB26E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC74FFB0-FD5F-4688-9158-105C85B650F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13980" windowHeight="7965" xr2:uid="{6CA504DF-EEC1-406B-8211-12A36D5258A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CA504DF-EEC1-406B-8211-12A36D5258A3}"/>
   </bookViews>
   <sheets>
     <sheet name="BVT" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>S no</t>
   </si>
@@ -270,6 +270,21 @@
 6. Zone 1 color will be set to 'yellow'
 7. Zone 1 value will be set to '378000'
 8. Zone 1 color will be set to 'yellow'</t>
+  </si>
+  <si>
+    <t>Basic Chart</t>
+  </si>
+  <si>
+    <t>1. Drag 'Revenue' in 'Actual Value' field.</t>
+  </si>
+  <si>
+    <t>Visual should be rendered for Revenue value.</t>
+  </si>
+  <si>
+    <t>1. Drag same value in all field.</t>
+  </si>
+  <si>
+    <t>Visual should be rendered properly.</t>
   </si>
 </sst>
 </file>
@@ -334,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -345,8 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -364,9 +378,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,19 +695,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89ECC3-919A-4CE0-A09A-814B2A8DA1B6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="21.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="49.140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="33.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -701,16 +715,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -718,60 +732,60 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="161.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="8"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -779,34 +793,68 @@
       <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +897,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -860,7 +908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -871,7 +919,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -904,7 +952,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -926,7 +974,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -937,7 +985,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -948,7 +996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1003,7 +1051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1024,7 +1072,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -1035,7 +1083,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -1061,7 +1109,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>19</v>
       </c>
@@ -1072,7 +1120,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>20</v>
       </c>

</xml_diff>